<commit_message>
More data for optimized helicopter
</commit_message>
<xml_diff>
--- a/Midterm Project/DropData.xlsx
+++ b/Midterm Project/DropData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>width</t>
   </si>
@@ -49,13 +49,19 @@
   <si>
     <t>Vel</t>
   </si>
+  <si>
+    <t>After Optimizing</t>
+  </si>
+  <si>
+    <t>same as above</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -97,7 +103,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -413,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F60581-C82B-450D-9236-5D2F41A53F38}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G12"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,6 +908,91 @@
         <v>9.25</v>
       </c>
     </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2.875</v>
+      </c>
+      <c r="B14">
+        <v>4.75</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="E14">
+        <v>1.86</v>
+      </c>
+      <c r="F14">
+        <v>2.13</v>
+      </c>
+      <c r="I14">
+        <v>15.5</v>
+      </c>
+      <c r="J14">
+        <v>5.25</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="E15">
+        <v>2.1</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5.5</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16">
+        <v>1.8</v>
+      </c>
+      <c r="E16">
+        <v>2.11</v>
+      </c>
+      <c r="F16">
+        <v>1.83</v>
+      </c>
+      <c r="I16">
+        <v>27.5</v>
+      </c>
+      <c r="J16">
+        <v>9</v>
+      </c>
+      <c r="K16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Final DoE Project Report
</commit_message>
<xml_diff>
--- a/Midterm Project/DropData.xlsx
+++ b/Midterm Project/DropData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{D42B615E-6F8F-4FAE-8020-CC75AB5A47B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1" xr2:uid="{D42B615E-6F8F-4FAE-8020-CC75AB5A47B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>width</t>
   </si>
@@ -54,6 +55,66 @@
   </si>
   <si>
     <t>same as above</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>−−−</t>
+  </si>
+  <si>
+    <t>−++</t>
+  </si>
+  <si>
+    <t>+−+</t>
+  </si>
+  <si>
+    <t>++−</t>
+  </si>
+  <si>
+    <t>−−+</t>
+  </si>
+  <si>
+    <t>+++</t>
+  </si>
+  <si>
+    <t>+−−</t>
+  </si>
+  <si>
+    <t>−+−</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>RotorWidth</t>
+  </si>
+  <si>
+    <t>Rotor Length</t>
+  </si>
+  <si>
+    <t>Nose Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance </t>
+  </si>
+  <si>
+    <t>Pred Formula Velocity</t>
+  </si>
+  <si>
+    <t>Pred Formula Distance</t>
   </si>
 </sst>
 </file>
@@ -120,6 +181,44 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E837068A-03F5-40BA-810B-0B31BE4108A5}" name="Table2" displayName="Table2" ref="A1:L16" totalsRowShown="0">
+  <autoFilter ref="A1:L16" xr:uid="{ACAF47C1-4DF0-40FA-9364-6577AC75CE68}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{39CACCF2-B3D2-4E1C-AAF5-28C40DD2E2B7}" name="width"/>
+    <tableColumn id="2" xr3:uid="{56D31279-FD54-48F9-AE4D-B4D3908C053A}" name="length"/>
+    <tableColumn id="3" xr3:uid="{4CBDE302-04BA-49B7-84F8-38F2382C3403}" name="nose"/>
+    <tableColumn id="4" xr3:uid="{9550626C-9A5B-4F27-A451-587282BF182A}" name="time"/>
+    <tableColumn id="5" xr3:uid="{7E0FC4CC-07B3-4739-938D-682C492717F2}" name="Column1"/>
+    <tableColumn id="6" xr3:uid="{62DE5D99-DECC-495B-AFC7-F766EB455151}" name="Column2"/>
+    <tableColumn id="7" xr3:uid="{C8E5CF94-72E3-4F5C-86FA-5B6E4A3ECC1E}" name="Vel"/>
+    <tableColumn id="8" xr3:uid="{16EEBE36-417B-486B-8BC1-797A240D0B2E}" name="MeanTime"/>
+    <tableColumn id="9" xr3:uid="{F417F04D-DF99-44AA-B562-97B25C0F19A6}" name="distance"/>
+    <tableColumn id="10" xr3:uid="{0756132E-3324-46B4-8FDC-D4B7C08C0A82}" name="Column3"/>
+    <tableColumn id="11" xr3:uid="{FCAC2B54-0CDE-4140-8288-254F6EC57E19}" name="Column4"/>
+    <tableColumn id="12" xr3:uid="{FAD4E2C9-6AE9-4746-9177-FE6D6E600F24}" name="MeanDist"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CD7E1376-DEB0-4BBB-A536-0F0FDC6A0427}" name="Table3" displayName="Table3" ref="A1:H12" totalsRowShown="0">
+  <autoFilter ref="A1:H12" xr:uid="{E8731162-E09D-45F9-8868-DA228496D49C}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{BD02E851-0E8D-4405-9E10-8E47A8D51492}" name="Pattern"/>
+    <tableColumn id="2" xr3:uid="{F4C50E6B-CFC4-478E-88C1-9454CA50A94B}" name="RotorWidth"/>
+    <tableColumn id="3" xr3:uid="{7A5A2340-A722-4C22-BD15-0B5D1272109F}" name="Rotor Length"/>
+    <tableColumn id="4" xr3:uid="{24BCD01D-6AC1-4C7A-9BBF-35FFD1949475}" name="Nose Length"/>
+    <tableColumn id="5" xr3:uid="{9739A7B1-B92C-43E4-9C31-7FCF950BA1AB}" name="Velocity "/>
+    <tableColumn id="6" xr3:uid="{95F545DE-7E79-41E0-90EF-D52908BC90BA}" name="Distance "/>
+    <tableColumn id="7" xr3:uid="{A0C9E46F-B3CD-42C9-8F0A-3BC32B453C63}" name="Pred Formula Velocity"/>
+    <tableColumn id="8" xr3:uid="{0D1E8E48-7245-48B1-963F-B52708B6CF65}" name="Pred Formula Distance"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,16 +518,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F60581-C82B-450D-9236-5D2F41A53F38}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -444,6 +546,12 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
       <c r="G1" t="s">
         <v>7</v>
       </c>
@@ -452,6 +560,12 @@
       </c>
       <c r="I1" t="s">
         <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
       </c>
       <c r="L1" t="s">
         <v>6</v>
@@ -518,11 +632,11 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G12" si="0">120/H3</f>
+        <f t="shared" ref="G3:G16" si="0">120/H3</f>
         <v>103.7463976945245</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H12" si="1">AVERAGE(D3:F3)</f>
+        <f t="shared" ref="H3:H16" si="1">AVERAGE(D3:F3)</f>
         <v>1.1566666666666665</v>
       </c>
       <c r="I3">
@@ -535,7 +649,7 @@
         <v>35</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L12" si="2">AVERAGE(I3:K3)</f>
+        <f t="shared" ref="L3:L16" si="2">AVERAGE(I3:K3)</f>
         <v>30.666666666666668</v>
       </c>
     </row>
@@ -912,6 +1026,18 @@
       <c r="A13" t="s">
         <v>8</v>
       </c>
+      <c r="G13" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L13" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -932,6 +1058,14 @@
       <c r="F14">
         <v>2.13</v>
       </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>59.800664451827252</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0066666666666664</v>
+      </c>
       <c r="I14">
         <v>15.5</v>
       </c>
@@ -940,6 +1074,10 @@
       </c>
       <c r="K14">
         <v>13</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="2"/>
+        <v>11.25</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -952,11 +1090,23 @@
       <c r="E15">
         <v>2.1</v>
       </c>
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>57.831325301204814</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0750000000000002</v>
+      </c>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15">
         <v>5</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -978,6 +1128,14 @@
       <c r="F16">
         <v>1.83</v>
       </c>
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
+        <v>62.717770034843205</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9133333333333333</v>
+      </c>
       <c r="I16">
         <v>27.5</v>
       </c>
@@ -987,14 +1145,356 @@
       <c r="K16">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
+      <c r="L16" s="3">
+        <f t="shared" si="2"/>
+        <v>19.166666666666668</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BE6F13-05B8-43F0-8B61-FFD5C8711D42}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>87.17</v>
+      </c>
+      <c r="F2">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="G2">
+        <v>82.385454545000002</v>
+      </c>
+      <c r="H2">
+        <v>10.872857142999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>1.5</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>103.75</v>
+      </c>
+      <c r="F3">
+        <v>30.67</v>
+      </c>
+      <c r="G3">
+        <v>96.230454545000001</v>
+      </c>
+      <c r="H3">
+        <v>21.93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>4.25</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>63.94</v>
+      </c>
+      <c r="F4">
+        <v>11.67</v>
+      </c>
+      <c r="G4">
+        <v>62.645454545</v>
+      </c>
+      <c r="H4">
+        <v>10.872857142999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>4.25</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>54.88</v>
+      </c>
+      <c r="F5">
+        <v>26.83</v>
+      </c>
+      <c r="G5">
+        <v>48.800454545000001</v>
+      </c>
+      <c r="H5">
+        <v>21.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>2.875</v>
+      </c>
+      <c r="C6">
+        <v>4.75</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>79.12</v>
+      </c>
+      <c r="F6">
+        <v>6.17</v>
+      </c>
+      <c r="G6">
+        <v>72.515454544999997</v>
+      </c>
+      <c r="H6">
+        <v>17.322857143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>1.5</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>99.72</v>
+      </c>
+      <c r="F7">
+        <v>14.25</v>
+      </c>
+      <c r="G7">
+        <v>96.230454545000001</v>
+      </c>
+      <c r="H7">
+        <v>10.872857142999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>4.25</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>63.05</v>
+      </c>
+      <c r="F8">
+        <v>25.17</v>
+      </c>
+      <c r="G8">
+        <v>62.645454545</v>
+      </c>
+      <c r="H8">
+        <v>21.93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>4.25</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>53.73</v>
+      </c>
+      <c r="F9">
+        <v>13.17</v>
+      </c>
+      <c r="G9">
+        <v>48.800454545000001</v>
+      </c>
+      <c r="H9">
+        <v>10.872857142999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>1.5</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>79.3</v>
+      </c>
+      <c r="F10">
+        <v>21.75</v>
+      </c>
+      <c r="G10">
+        <v>82.385454545000002</v>
+      </c>
+      <c r="H10">
+        <v>21.93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>2.875</v>
+      </c>
+      <c r="C11">
+        <v>4.75</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>51.58</v>
+      </c>
+      <c r="F11">
+        <v>7.92</v>
+      </c>
+      <c r="G11">
+        <v>72.515454544999997</v>
+      </c>
+      <c r="H11">
+        <v>17.322857143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>2.875</v>
+      </c>
+      <c r="C12">
+        <v>4.75</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>61.43</v>
+      </c>
+      <c r="F12">
+        <v>9.25</v>
+      </c>
+      <c r="G12">
+        <v>72.515454544999997</v>
+      </c>
+      <c r="H12">
+        <v>17.322857143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>